<commit_message>
Update Jan16_a_ Ago18_cartoes ativos BOM.xlsx
</commit_message>
<xml_diff>
--- a/data/Jan16_a_ Ago18_cartoes ativos BOM.xlsx
+++ b/data/Jan16_a_ Ago18_cartoes ativos BOM.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26821"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2689E92F-7CA0-4DFD-982C-EDF9CD653AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4020" windowWidth="20520" windowHeight="4080"/>
+    <workbookView xWindow="-15" yWindow="4020" windowWidth="20520" windowHeight="4080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RMSP" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>MÊS</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
   <si>
     <t>HISTÓRICO DA QUANTIDADE DE CARTÕES ATIVOS - RMSP</t>
   </si>
@@ -29,6 +37,9 @@
   </si>
   <si>
     <t>Fonte: Autopass - Relatório QUANTIDADE DE CARTÕES - SINTÉTICO (RPT)</t>
+  </si>
+  <si>
+    <t>MÊS</t>
   </si>
   <si>
     <t>VT</t>
@@ -43,19 +54,22 @@
     <t>Empresarial</t>
   </si>
   <si>
+    <t>Sênior</t>
+  </si>
+  <si>
     <t>Especial</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>Observações:</t>
   </si>
   <si>
-    <t>Sênior</t>
+    <t>a. Escolar - Cartão que inclui as aplicações Meia Tarifa e Passe Livre.</t>
   </si>
   <si>
     <t>b. Sênior - Cartão que inclui as aplicações Sênior Paulista (60/64) e Sênior (65+).</t>
-  </si>
-  <si>
-    <t>a. Escolar - Cartão que inclui as aplicações Meia Tarifa e Passe Livre.</t>
   </si>
   <si>
     <t>c. Dados obtidos entre os dias 1 e 5 do mês subsequente.</t>
@@ -64,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +187,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -290,7 +307,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -474,53 +491,53 @@
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="H3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>42370</v>
       </c>
@@ -547,7 +564,7 @@
         <v>4857310</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>42401</v>
       </c>
@@ -574,7 +591,7 @@
         <v>4903426</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>42430</v>
       </c>
@@ -601,7 +618,7 @@
         <v>4954840</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>42461</v>
       </c>
@@ -628,7 +645,7 @@
         <v>5008918</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>42491</v>
       </c>
@@ -655,7 +672,7 @@
         <v>5045836</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>42522</v>
       </c>
@@ -682,7 +699,7 @@
         <v>5010903</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>42552</v>
       </c>
@@ -709,7 +726,7 @@
         <v>5046461</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>42583</v>
       </c>
@@ -736,7 +753,7 @@
         <v>5150885</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>42614</v>
       </c>
@@ -763,7 +780,7 @@
         <v>5185383</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>42644</v>
       </c>
@@ -790,7 +807,7 @@
         <v>5208059</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>42675</v>
       </c>
@@ -817,7 +834,7 @@
         <v>5213843</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>42705</v>
       </c>
@@ -844,7 +861,7 @@
         <v>5260919</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>42736</v>
       </c>
@@ -871,7 +888,7 @@
         <v>5304152</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>42767</v>
       </c>
@@ -898,7 +915,7 @@
         <v>5339116</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>42795</v>
       </c>
@@ -925,7 +942,7 @@
         <v>5384252</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>42826</v>
       </c>
@@ -952,7 +969,7 @@
         <v>5449318</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>42856</v>
       </c>
@@ -979,7 +996,7 @@
         <v>5504871</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>42887</v>
       </c>
@@ -1006,7 +1023,7 @@
         <v>5512971</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>42917</v>
       </c>
@@ -1033,7 +1050,7 @@
         <v>5617773</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>42948</v>
       </c>
@@ -1060,7 +1077,7 @@
         <v>5694398</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>42979</v>
       </c>
@@ -1087,7 +1104,7 @@
         <v>5765374</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>43009</v>
       </c>
@@ -1114,7 +1131,7 @@
         <v>5814329</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>43040</v>
       </c>
@@ -1141,7 +1158,7 @@
         <v>5815915</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
         <v>43070</v>
       </c>
@@ -1168,7 +1185,7 @@
         <v>5901731</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
         <v>43101</v>
       </c>
@@ -1195,7 +1212,7 @@
         <v>5939744</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
         <v>43132</v>
       </c>
@@ -1222,7 +1239,7 @@
         <v>5980231</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
         <v>43160</v>
       </c>
@@ -1249,7 +1266,7 @@
         <v>6032579</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>43191</v>
       </c>
@@ -1276,7 +1293,7 @@
         <v>6078047</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>43221</v>
       </c>
@@ -1303,7 +1320,7 @@
         <v>6123848</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="2">
         <v>43252</v>
       </c>
@@ -1330,7 +1347,7 @@
         <v>6159488</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>43282</v>
       </c>
@@ -1357,7 +1374,7 @@
         <v>6203030</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
         <v>43313</v>
       </c>
@@ -1384,7 +1401,7 @@
         <v>6253336</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1394,9 +1411,9 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1406,17 +1423,17 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="8" t="s">
         <v>14</v>
       </c>

</xml_diff>